<commit_message>
form hand seal finished
</commit_message>
<xml_diff>
--- a/Onmyoji Modifiers.xlsx
+++ b/Onmyoji Modifiers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEACA99-FA85-4E19-80E8-03F8473449BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E072FB8-DA52-48DC-A9E0-077EA7CBEEC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
   </bookViews>
@@ -1241,7 +1241,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,7 +1351,7 @@
         <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>78</v>
@@ -1367,14 +1367,14 @@
       </c>
       <c r="C8" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C7,Sheet1!L$3:L$38,0))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="I8" t="str">
         <f>_xlfn.CONCAT(A8:F8)</f>
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dodge, ward, and take hit
</commit_message>
<xml_diff>
--- a/Onmyoji Modifiers.xlsx
+++ b/Onmyoji Modifiers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E072FB8-DA52-48DC-A9E0-077EA7CBEEC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F28FB1D-135C-44F6-87E5-AB135FA3B964}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
   </bookViews>
@@ -1241,7 +1241,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,7 +1317,7 @@
         <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>78</v>
@@ -1331,16 +1331,16 @@
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(B5,Sheet1!I$3:I$38,0))</f>
         <v>1</v>
       </c>
-      <c r="C6" s="8" t="str">
+      <c r="C6" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C5,Sheet1!J$3:J$38,0))</f>
-        <v>Z</v>
+        <v>0</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="I6" t="str">
         <f>_xlfn.CONCAT(A6:F6)</f>
-        <v>21Z</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
projectile effect with working crit
</commit_message>
<xml_diff>
--- a/Onmyoji Modifiers.xlsx
+++ b/Onmyoji Modifiers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F28FB1D-135C-44F6-87E5-AB135FA3B964}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B3E6DF-B3BA-4BD1-B140-76744B0183AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
+    <workbookView xWindow="14325" yWindow="2775" windowWidth="12825" windowHeight="12825" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1241,7 +1241,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,19 +1262,19 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>78</v>
@@ -1284,29 +1284,29 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="8" t="str">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(B3,Sheet1!C$3:C$38,0))</f>
-        <v>2</v>
+        <v>Z</v>
       </c>
       <c r="C4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C3,Sheet1!D$3:D$38,0))</f>
-        <v>2</v>
-      </c>
-      <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8" t="str">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(D3,Sheet1!E$3:E$38,0))</f>
-        <v>4</v>
+        <v>Z</v>
       </c>
       <c r="E4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(E3,Sheet1!F$3:F$38,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="8">
+        <v>6</v>
+      </c>
+      <c r="F4" s="8" t="str">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(F3,Sheet1!G$3:G$38,0))</f>
-        <v>0</v>
+        <v>Z</v>
       </c>
       <c r="I4" t="str">
         <f>_xlfn.CONCAT(A4:F4)</f>
-        <v>122400</v>
+        <v>1Z1Z6Z</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finish body graphic, living spells working
</commit_message>
<xml_diff>
--- a/Onmyoji Modifiers.xlsx
+++ b/Onmyoji Modifiers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B3E6DF-B3BA-4BD1-B140-76744B0183AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9902A79-A4F4-43C4-8384-6F5A49068E02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14325" yWindow="2775" windowWidth="12825" windowHeight="12825" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1241,7 +1241,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,19 +1262,19 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>78</v>
@@ -1284,29 +1284,29 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="str">
+      <c r="B4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(B3,Sheet1!C$3:C$38,0))</f>
-        <v>Z</v>
+        <v>2</v>
       </c>
       <c r="C4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C3,Sheet1!D$3:D$38,0))</f>
-        <v>1</v>
-      </c>
-      <c r="D4" s="8" t="str">
+        <v>3</v>
+      </c>
+      <c r="D4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(D3,Sheet1!E$3:E$38,0))</f>
-        <v>Z</v>
+        <v>2</v>
       </c>
       <c r="E4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(E3,Sheet1!F$3:F$38,0))</f>
-        <v>6</v>
-      </c>
-      <c r="F4" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(F3,Sheet1!G$3:G$38,0))</f>
-        <v>Z</v>
+        <v>0</v>
       </c>
       <c r="I4" t="str">
         <f>_xlfn.CONCAT(A4:F4)</f>
-        <v>1Z1Z6Z</v>
+        <v>123210</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
area targeting working, effect wip
</commit_message>
<xml_diff>
--- a/Onmyoji Modifiers.xlsx
+++ b/Onmyoji Modifiers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9902A79-A4F4-43C4-8384-6F5A49068E02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B230C99-1901-4641-9129-D1549CD1D4BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
   </bookViews>
@@ -1241,7 +1241,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,19 +1262,19 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="E3" t="s">
         <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>78</v>
@@ -1284,29 +1284,29 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="8" t="str">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(B3,Sheet1!C$3:C$38,0))</f>
-        <v>2</v>
+        <v>Z</v>
       </c>
       <c r="C4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C3,Sheet1!D$3:D$38,0))</f>
-        <v>3</v>
-      </c>
-      <c r="D4" s="8">
+        <v>2</v>
+      </c>
+      <c r="D4" s="8" t="str">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(D3,Sheet1!E$3:E$38,0))</f>
-        <v>2</v>
+        <v>Z</v>
       </c>
       <c r="E4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(E3,Sheet1!F$3:F$38,0))</f>
         <v>1</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="8" t="str">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(F3,Sheet1!G$3:G$38,0))</f>
-        <v>0</v>
+        <v>Z</v>
       </c>
       <c r="I4" t="str">
         <f>_xlfn.CONCAT(A4:F4)</f>
-        <v>123210</v>
+        <v>1Z2Z1Z</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
auto damage for players
</commit_message>
<xml_diff>
--- a/Onmyoji Modifiers.xlsx
+++ b/Onmyoji Modifiers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72DBCE4-89F9-4B4B-9650-B9847DF0D5CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221CC41E-7837-47B8-B51A-68191B87AEFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -731,7 +731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25B2E206-CE3A-441E-9767-B84A47E2A9DA}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -1252,8 +1252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8DFB6C6-09DB-4B15-801E-5605D6167238}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,7 +1283,7 @@
         <v>77</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="F3" t="s">
         <v>90</v>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="E4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(E3,Sheet1!F$3:F$38,0))</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(F3,Sheet1!G$3:G$38,0))</f>
@@ -1318,7 +1318,7 @@
       </c>
       <c r="I4" t="str">
         <f>_xlfn.CONCAT(A4:F4)</f>
-        <v>1Z2Z16</v>
+        <v>1Z2Z66</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
auto damage updated on living spell
</commit_message>
<xml_diff>
--- a/Onmyoji Modifiers.xlsx
+++ b/Onmyoji Modifiers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221CC41E-7837-47B8-B51A-68191B87AEFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB04F2E-6293-4516-A6B0-AFD6D0981C50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
   </bookViews>
@@ -1253,7 +1253,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:F3"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1274,19 +1274,19 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F3" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>78</v>
@@ -1296,29 +1296,29 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="str">
+      <c r="B4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(B3,Sheet1!C$3:C$38,0))</f>
-        <v>Z</v>
+        <v>1</v>
       </c>
       <c r="C4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C3,Sheet1!D$3:D$38,0))</f>
-        <v>2</v>
-      </c>
-      <c r="D4" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(D3,Sheet1!E$3:E$38,0))</f>
-        <v>Z</v>
+        <v>6</v>
       </c>
       <c r="E4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(E3,Sheet1!F$3:F$38,0))</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(F3,Sheet1!G$3:G$38,0))</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I4" t="str">
         <f>_xlfn.CONCAT(A4:F4)</f>
-        <v>1Z2Z66</v>
+        <v>111600</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
binding spells added. version 0.2
</commit_message>
<xml_diff>
--- a/Onmyoji Modifiers.xlsx
+++ b/Onmyoji Modifiers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB04F2E-6293-4516-A6B0-AFD6D0981C50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659947F1-A6C4-4976-832D-971A55CD48C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
   </bookViews>
@@ -1274,19 +1274,19 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
         <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>78</v>
@@ -1296,13 +1296,13 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="8" t="str">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(B3,Sheet1!C$3:C$38,0))</f>
-        <v>1</v>
-      </c>
-      <c r="C4" s="8">
+        <v>Z</v>
+      </c>
+      <c r="C4" s="8" t="str">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C3,Sheet1!D$3:D$38,0))</f>
-        <v>1</v>
+        <v>Z</v>
       </c>
       <c r="D4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(D3,Sheet1!E$3:E$38,0))</f>
@@ -1310,15 +1310,15 @@
       </c>
       <c r="E4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(E3,Sheet1!F$3:F$38,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8" t="str">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(F3,Sheet1!G$3:G$38,0))</f>
-        <v>0</v>
+        <v>Z</v>
       </c>
       <c r="I4" t="str">
         <f>_xlfn.CONCAT(A4:F4)</f>
-        <v>111600</v>
+        <v>1ZZ61Z</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
exorcism casting works, need to check damaging
</commit_message>
<xml_diff>
--- a/Onmyoji Modifiers.xlsx
+++ b/Onmyoji Modifiers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659947F1-A6C4-4976-832D-971A55CD48C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9642AFA5-D055-4A92-AE70-8E180681FD59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="95">
   <si>
     <t>Attack</t>
   </si>
@@ -311,6 +311,15 @@
   </si>
   <si>
     <t>Cancel</t>
+  </si>
+  <si>
+    <t>Exorcism</t>
+  </si>
+  <si>
+    <t>Bind</t>
+  </si>
+  <si>
+    <t>Drain</t>
   </si>
 </sst>
 </file>
@@ -732,15 +741,14 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="5"/>
     <col min="3" max="3" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" customWidth="1"/>
@@ -1002,6 +1010,9 @@
       <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="D8" t="s">
+        <v>92</v>
+      </c>
       <c r="E8" t="s">
         <v>22</v>
       </c>
@@ -1031,6 +1042,9 @@
       <c r="A9" s="5">
         <v>5</v>
       </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
       <c r="E9" t="s">
         <v>23</v>
       </c>
@@ -1060,8 +1074,11 @@
       <c r="A10" s="5">
         <v>6</v>
       </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="F10" t="s">
         <v>81</v>
@@ -1083,8 +1100,11 @@
       <c r="A11" s="5">
         <v>7</v>
       </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>91</v>
@@ -1097,24 +1117,21 @@
       <c r="A12" s="5">
         <v>8</v>
       </c>
+      <c r="D12" t="s">
+        <v>89</v>
+      </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>9</v>
       </c>
-      <c r="E13" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="E14" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1253,7 +1270,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1274,19 +1291,19 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>94</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>78</v>
@@ -1296,29 +1313,29 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="str">
+      <c r="B4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(B3,Sheet1!C$3:C$38,0))</f>
-        <v>Z</v>
-      </c>
-      <c r="C4" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C3,Sheet1!D$3:D$38,0))</f>
-        <v>Z</v>
+        <v>4</v>
       </c>
       <c r="D4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(D3,Sheet1!E$3:E$38,0))</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(E3,Sheet1!F$3:F$38,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="8" t="str">
+        <v>3</v>
+      </c>
+      <c r="F4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(F3,Sheet1!G$3:G$38,0))</f>
-        <v>Z</v>
+        <v>0</v>
       </c>
       <c r="I4" t="str">
         <f>_xlfn.CONCAT(A4:F4)</f>
-        <v>1ZZ61Z</v>
+        <v>114830</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1400,18 +1417,6 @@
             <xm:f>Sheet1!$C$3:$C$38</xm:f>
           </x14:formula1>
           <xm:sqref>B3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FC1C38F2-C32E-4ABC-869B-CF2AB3D80B48}">
-          <x14:formula1>
-            <xm:f>Sheet1!$D$3:$D$38</xm:f>
-          </x14:formula1>
-          <xm:sqref>C3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6EEAC295-002E-4840-8FB4-5E6CD87D035B}">
-          <x14:formula1>
-            <xm:f>Sheet1!$E$3:$E$38</xm:f>
-          </x14:formula1>
-          <xm:sqref>D3 D5 D7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D28E1B9C-4EAC-47EB-B63E-8B08534C473A}">
           <x14:formula1>
@@ -1449,6 +1454,18 @@
           </x14:formula1>
           <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FC1C38F2-C32E-4ABC-869B-CF2AB3D80B48}">
+          <x14:formula1>
+            <xm:f>Sheet1!$D$3:$D$38</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6EEAC295-002E-4840-8FB4-5E6CD87D035B}">
+          <x14:formula1>
+            <xm:f>Sheet1!$E$3:$E$38</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3 D5 D7</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Counter reaction working and crits tracked per token
</commit_message>
<xml_diff>
--- a/Onmyoji Modifiers.xlsx
+++ b/Onmyoji Modifiers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9642AFA5-D055-4A92-AE70-8E180681FD59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FE6C47-67C7-4CCA-AC18-D1E336F44C13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="93">
   <si>
     <t>Attack</t>
   </si>
@@ -151,24 +151,12 @@
     <t>Dodge</t>
   </si>
   <si>
-    <t>Endure Injury</t>
-  </si>
-  <si>
-    <t>Armor</t>
-  </si>
-  <si>
-    <t>Counterspell</t>
-  </si>
-  <si>
     <t>Take Hit</t>
   </si>
   <si>
     <t>Spirit Recover</t>
   </si>
   <si>
-    <t>Multi-User Barrier</t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
@@ -320,6 +308,12 @@
   </si>
   <si>
     <t>Drain</t>
+  </si>
+  <si>
+    <t>Counter</t>
+  </si>
+  <si>
+    <t>Full Defense Dodge</t>
   </si>
 </sst>
 </file>
@@ -392,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -424,6 +418,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,7 +736,7 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,7 +747,7 @@
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
@@ -798,13 +793,13 @@
         <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>9</v>
@@ -818,75 +813,75 @@
         <v>0</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="L4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -912,7 +907,7 @@
         <v>31</v>
       </c>
       <c r="H5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>37</v>
@@ -921,7 +916,7 @@
         <v>30</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="L5" t="s">
         <v>30</v>
@@ -950,7 +945,7 @@
         <v>32</v>
       </c>
       <c r="H6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>38</v>
@@ -959,7 +954,7 @@
         <v>28</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>
@@ -988,16 +983,16 @@
         <v>33</v>
       </c>
       <c r="H7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="J7" t="s">
         <v>29</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="L7" t="s">
         <v>29</v>
@@ -1011,7 +1006,7 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E8" t="s">
         <v>22</v>
@@ -1023,16 +1018,16 @@
         <v>34</v>
       </c>
       <c r="H8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J8" t="s">
         <v>11</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L8" t="s">
         <v>11</v>
@@ -1055,16 +1050,13 @@
         <v>35</v>
       </c>
       <c r="H9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="J9" t="s">
         <v>36</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="L9" t="s">
         <v>36</v>
@@ -1078,22 +1070,19 @@
         <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H10" t="s">
-        <v>88</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1107,10 +1096,7 @@
         <v>26</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>43</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1118,10 +1104,13 @@
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E12" t="s">
-        <v>94</v>
+        <v>90</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1131,127 +1120,127 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1270,7 +1259,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,7 +1272,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1291,51 +1280,51 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="8" t="str">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(B3,Sheet1!C$3:C$38,0))</f>
-        <v>1</v>
-      </c>
-      <c r="C4" s="8">
+        <v>Z</v>
+      </c>
+      <c r="C4" s="8" t="str">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C3,Sheet1!D$3:D$38,0))</f>
-        <v>4</v>
-      </c>
-      <c r="D4" s="8">
+        <v>Z</v>
+      </c>
+      <c r="D4" s="8" t="str">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(D3,Sheet1!E$3:E$38,0))</f>
-        <v>8</v>
+        <v>Z</v>
       </c>
       <c r="E4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(E3,Sheet1!F$3:F$38,0))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(F3,Sheet1!G$3:G$38,0))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I4" t="str">
         <f>_xlfn.CONCAT(A4:F4)</f>
-        <v>114830</v>
+        <v>1ZZZ18</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1343,13 +1332,13 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1358,7 +1347,7 @@
       </c>
       <c r="B6" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(B5,Sheet1!I$3:I$38,0))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C5,Sheet1!J$3:J$38,0))</f>
@@ -1369,7 +1358,7 @@
       <c r="F6" s="8"/>
       <c r="I6" t="str">
         <f>_xlfn.CONCAT(A6:F6)</f>
-        <v>210</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1377,13 +1366,13 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1423,12 +1412,6 @@
             <xm:f>Sheet1!$F$3:$F$38</xm:f>
           </x14:formula1>
           <xm:sqref>E3 E5 E7</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BCEBAAE2-5EE6-47DF-9EA3-230757E32871}">
-          <x14:formula1>
-            <xm:f>Sheet1!$I$3:$I$38</xm:f>
-          </x14:formula1>
-          <xm:sqref>B5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{09FA6813-55F0-4F96-A497-171B14AE93F4}">
           <x14:formula1>
@@ -1466,6 +1449,12 @@
           </x14:formula1>
           <xm:sqref>D3 D5 D7</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BCEBAAE2-5EE6-47DF-9EA3-230757E32871}">
+          <x14:formula1>
+            <xm:f>Sheet1!$I$3:$I$38</xm:f>
+          </x14:formula1>
+          <xm:sqref>B5</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
stealth spell casting, channel and cancel
</commit_message>
<xml_diff>
--- a/Onmyoji Modifiers.xlsx
+++ b/Onmyoji Modifiers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FE6C47-67C7-4CCA-AC18-D1E336F44C13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31E4C2D-A4E5-4DEB-9A0A-32273CF9B87C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
   </bookViews>
@@ -406,6 +406,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -418,7 +419,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,7 +736,7 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,29 +754,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
       <c r="H1" s="12"/>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="16"/>
-      <c r="K1" s="15" t="s">
+      <c r="J1" s="17"/>
+      <c r="K1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="16"/>
+      <c r="L1" s="17"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="14"/>
+      <c r="B2" s="15"/>
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
         <v>89</v>
@@ -1090,26 +1090,26 @@
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="E11" t="s">
         <v>26</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>87</v>
+      </c>
+      <c r="K11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>8</v>
       </c>
-      <c r="D12" t="s">
-        <v>85</v>
-      </c>
       <c r="E12" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1259,7 +1259,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1366,7 +1366,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
         <v>75</v>
@@ -1381,7 +1381,7 @@
       </c>
       <c r="B8" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(B7,Sheet1!K$3:K$38,0))</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C7,Sheet1!L$3:L$38,0))</f>
@@ -1392,7 +1392,7 @@
       <c r="F8" s="8"/>
       <c r="I8" t="str">
         <f>_xlfn.CONCAT(A8:F8)</f>
-        <v>360</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -1431,6 +1431,18 @@
           </x14:formula1>
           <xm:sqref>F3 F7 F5</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6EEAC295-002E-4840-8FB4-5E6CD87D035B}">
+          <x14:formula1>
+            <xm:f>Sheet1!$E$3:$E$38</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3 D5 D7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BCEBAAE2-5EE6-47DF-9EA3-230757E32871}">
+          <x14:formula1>
+            <xm:f>Sheet1!$I$3:$I$38</xm:f>
+          </x14:formula1>
+          <xm:sqref>B5</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{24297926-D19A-4074-95E4-8EB52B5E1440}">
           <x14:formula1>
             <xm:f>Sheet1!$K$3:$K$38</xm:f>
@@ -1443,18 +1455,6 @@
           </x14:formula1>
           <xm:sqref>C3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6EEAC295-002E-4840-8FB4-5E6CD87D035B}">
-          <x14:formula1>
-            <xm:f>Sheet1!$E$3:$E$38</xm:f>
-          </x14:formula1>
-          <xm:sqref>D3 D5 D7</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BCEBAAE2-5EE6-47DF-9EA3-230757E32871}">
-          <x14:formula1>
-            <xm:f>Sheet1!$I$3:$I$38</xm:f>
-          </x14:formula1>
-          <xm:sqref>B5</xm:sqref>
-        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
reveal stealth via sense rolll
</commit_message>
<xml_diff>
--- a/Onmyoji Modifiers.xlsx
+++ b/Onmyoji Modifiers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C21703-172C-4038-A764-9812B3F459EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB07E6C6-06CE-435D-8DDC-5BCDEFFCC8B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
   </bookViews>
@@ -1366,10 +1366,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>74</v>
@@ -1381,18 +1381,18 @@
       </c>
       <c r="B8" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(B7,Sheet1!K$3:K$38,0))</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C8" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C7,Sheet1!L$3:L$38,0))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="I8" t="str">
         <f>_xlfn.CONCAT(A8:F8)</f>
-        <v>371</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
barrier casting and channeling
</commit_message>
<xml_diff>
--- a/Onmyoji Modifiers.xlsx
+++ b/Onmyoji Modifiers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB07E6C6-06CE-435D-8DDC-5BCDEFFCC8B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071ED749-31E3-4CE5-8FDE-7DC98E32D5FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
   </bookViews>
@@ -736,7 +736,7 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,6 +1052,9 @@
       <c r="H9" t="s">
         <v>83</v>
       </c>
+      <c r="I9" t="s">
+        <v>85</v>
+      </c>
       <c r="J9" t="s">
         <v>36</v>
       </c>
@@ -1088,9 +1091,6 @@
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>7</v>
-      </c>
-      <c r="D11" t="s">
-        <v>85</v>
       </c>
       <c r="E11" t="s">
         <v>26</v>
@@ -1259,7 +1259,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,10 +1280,10 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="D3" t="s">
         <v>73</v>
@@ -1302,13 +1302,13 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="str">
+      <c r="B4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(B3,Sheet1!C$3:C$38,0))</f>
-        <v>Z</v>
-      </c>
-      <c r="C4" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8" t="e">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C3,Sheet1!D$3:D$38,0))</f>
-        <v>Z</v>
+        <v>#N/A</v>
       </c>
       <c r="D4" s="8" t="str">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(D3,Sheet1!E$3:E$38,0))</f>
@@ -1322,9 +1322,9 @@
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(F3,Sheet1!G$3:G$38,0))</f>
         <v>6</v>
       </c>
-      <c r="I4" t="str">
+      <c r="I4" t="e">
         <f>_xlfn.CONCAT(A4:F4)</f>
-        <v>1ZZZ16</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1332,10 +1332,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>74</v>
@@ -1347,18 +1347,18 @@
       </c>
       <c r="B6" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(B5,Sheet1!I$3:I$38,0))</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C6" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C5,Sheet1!J$3:J$38,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="I6" t="str">
         <f>_xlfn.CONCAT(A6:F6)</f>
-        <v>230</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1437,17 +1437,17 @@
           </x14:formula1>
           <xm:sqref>D3 D5 D7</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{24297926-D19A-4074-95E4-8EB52B5E1440}">
+          <x14:formula1>
+            <xm:f>Sheet1!$K$3:$K$38</xm:f>
+          </x14:formula1>
+          <xm:sqref>B7</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BCEBAAE2-5EE6-47DF-9EA3-230757E32871}">
           <x14:formula1>
             <xm:f>Sheet1!$I$3:$I$38</xm:f>
           </x14:formula1>
           <xm:sqref>B5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{24297926-D19A-4074-95E4-8EB52B5E1440}">
-          <x14:formula1>
-            <xm:f>Sheet1!$K$3:$K$38</xm:f>
-          </x14:formula1>
-          <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FC1C38F2-C32E-4ABC-869B-CF2AB3D80B48}">
           <x14:formula1>

</xml_diff>

<commit_message>
spirit flow spells finished
</commit_message>
<xml_diff>
--- a/Onmyoji Modifiers.xlsx
+++ b/Onmyoji Modifiers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071ED749-31E3-4CE5-8FDE-7DC98E32D5FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A63636A-11CA-4A63-BE04-2F8B2EA6C25E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
   </bookViews>
@@ -1259,7 +1259,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,16 +1283,16 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="F3" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>74</v>
@@ -1306,25 +1306,25 @@
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(B3,Sheet1!C$3:C$38,0))</f>
         <v>1</v>
       </c>
-      <c r="C4" s="8" t="e">
+      <c r="C4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C3,Sheet1!D$3:D$38,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D4" s="8" t="str">
+        <v>6</v>
+      </c>
+      <c r="D4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(D3,Sheet1!E$3:E$38,0))</f>
-        <v>Z</v>
+        <v>8</v>
       </c>
       <c r="E4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(E3,Sheet1!F$3:F$38,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(F3,Sheet1!G$3:G$38,0))</f>
-        <v>6</v>
-      </c>
-      <c r="I4" t="e">
+        <v>0</v>
+      </c>
+      <c r="I4" t="str">
         <f>_xlfn.CONCAT(A4:F4)</f>
-        <v>#N/A</v>
+        <v>116800</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1332,7 +1332,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
         <v>30</v>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="B6" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(B5,Sheet1!I$3:I$38,0))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C5,Sheet1!J$3:J$38,0))</f>
@@ -1358,7 +1358,7 @@
       <c r="F6" s="8"/>
       <c r="I6" t="str">
         <f>_xlfn.CONCAT(A6:F6)</f>
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
rearrange image files # Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/Onmyoji Modifiers.xlsx
+++ b/Onmyoji Modifiers.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A63636A-11CA-4A63-BE04-2F8B2EA6C25E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E355F2E4-3A8C-4F2F-8CA2-3C7DAF5F4494}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="109">
   <si>
     <t>Attack</t>
   </si>
@@ -314,6 +315,54 @@
   </si>
   <si>
     <t>Full Defense Dodge</t>
+  </si>
+  <si>
+    <t>Compound</t>
+  </si>
+  <si>
+    <t>Compounding Outcomes</t>
+  </si>
+  <si>
+    <t>Consumed Spell</t>
+  </si>
+  <si>
+    <t>Cast Spell</t>
+  </si>
+  <si>
+    <t>Static</t>
+  </si>
+  <si>
+    <t>Generating</t>
+  </si>
+  <si>
+    <t>Remove old area, damage dealt on cast</t>
+  </si>
+  <si>
+    <t>Remove old living, damage dealt on cast</t>
+  </si>
+  <si>
+    <t>Remove old static, damage dealt on cast</t>
+  </si>
+  <si>
+    <t>Change area element, retain original owner</t>
+  </si>
+  <si>
+    <t>Change living element</t>
+  </si>
+  <si>
+    <t>Change area element, gain ownership</t>
+  </si>
+  <si>
+    <t>Cancelling (partial cancel)</t>
+  </si>
+  <si>
+    <t>Cast area cancelled</t>
+  </si>
+  <si>
+    <t>Projectile cancelled</t>
+  </si>
+  <si>
+    <t>Area casts, reduced per spell</t>
   </si>
 </sst>
 </file>
@@ -386,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -407,6 +456,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -417,6 +469,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -736,7 +791,7 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,29 +809,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
       <c r="H1" s="12"/>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="17"/>
-      <c r="K1" s="16" t="s">
+      <c r="J1" s="18"/>
+      <c r="K1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="17"/>
+      <c r="L1" s="18"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="15"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1116,6 +1171,9 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>9</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1258,8 +1316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8DFB6C6-09DB-4B15-801E-5605D6167238}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,4 +1517,122 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6593BB41-7EDA-4B01-963F-AFFAD10E97AD}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
configure new token as player or npc
</commit_message>
<xml_diff>
--- a/Onmyoji Modifiers.xlsx
+++ b/Onmyoji Modifiers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15DC341-23B5-4FBE-AF95-9C0B8ABFF8A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB51B50-45B8-4847-8A72-BE1DED79A0F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
   </bookViews>
@@ -1317,7 +1317,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1338,19 +1338,19 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>74</v>
@@ -1362,27 +1362,27 @@
       </c>
       <c r="B4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(B3,Sheet1!C$3:C$38,0))</f>
-        <v>2</v>
-      </c>
-      <c r="C4" s="8">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8" t="str">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C3,Sheet1!D$3:D$38,0))</f>
-        <v>1</v>
-      </c>
-      <c r="D4" s="8">
+        <v>Z</v>
+      </c>
+      <c r="D4" s="8" t="str">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(D3,Sheet1!E$3:E$38,0))</f>
-        <v>3</v>
+        <v>Z</v>
       </c>
       <c r="E4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(E3,Sheet1!F$3:F$38,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="8">
+        <v>3</v>
+      </c>
+      <c r="F4" s="8" t="str">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(F3,Sheet1!G$3:G$38,0))</f>
-        <v>0</v>
+        <v>Z</v>
       </c>
       <c r="I4" t="str">
         <f>_xlfn.CONCAT(A4:F4)</f>
-        <v>121300</v>
+        <v>11ZZ3Z</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
save turn info to handout for restart
</commit_message>
<xml_diff>
--- a/Onmyoji Modifiers.xlsx
+++ b/Onmyoji Modifiers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81530795-CDF3-4D2B-B8E0-AFA87EF95648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A9E406-0EAE-4D6A-8336-4CC2A52D52FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
   </bookViews>
@@ -1336,7 +1336,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1409,10 +1409,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>74</v>
@@ -1424,18 +1424,18 @@
       </c>
       <c r="B6" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(B5,Sheet1!I$3:I$38,0))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C5,Sheet1!J$3:J$38,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="I6" t="str">
         <f>_xlfn.CONCAT(A6:F6)</f>
-        <v>231</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
bonusStat working w/ toggle ability
</commit_message>
<xml_diff>
--- a/Onmyoji Modifiers.xlsx
+++ b/Onmyoji Modifiers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A9E406-0EAE-4D6A-8336-4CC2A52D52FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5CE3748-5D0D-4A1D-A9D3-48624D3F1B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
   </bookViews>
@@ -1336,7 +1336,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1366,7 +1366,7 @@
         <v>73</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
         <v>73</v>
@@ -1393,7 +1393,7 @@
       </c>
       <c r="E4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(E3,Sheet1!F$3:F$38,0))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" s="8" t="str">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(F3,Sheet1!G$3:G$38,0))</f>
@@ -1401,7 +1401,7 @@
       </c>
       <c r="I4" t="str">
         <f>_xlfn.CONCAT(A4:F4)</f>
-        <v>13ZZ6Z</v>
+        <v>13ZZ5Z</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add mods to initiative roll
</commit_message>
<xml_diff>
--- a/Onmyoji Modifiers.xlsx
+++ b/Onmyoji Modifiers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5CE3748-5D0D-4A1D-A9D3-48624D3F1B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2706ADB6-5674-4604-83D0-36E0002C7395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
   </bookViews>
@@ -800,7 +800,7 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,7 +1336,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1443,10 +1443,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>74</v>
@@ -1458,18 +1458,18 @@
       </c>
       <c r="B8" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(B7,Sheet1!K$3:K$38,0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C7,Sheet1!L$3:L$38,0))</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="I8" t="str">
         <f>_xlfn.CONCAT(A8:F8)</f>
-        <v>315</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixes for bonus damage
</commit_message>
<xml_diff>
--- a/Onmyoji Modifiers.xlsx
+++ b/Onmyoji Modifiers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2706ADB6-5674-4604-83D0-36E0002C7395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8C39DB-7443-4E50-BC83-52A54A0DE0B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="113">
   <si>
     <t>Attack</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Talisman</t>
   </si>
   <si>
-    <t>Enhancement</t>
-  </si>
-  <si>
     <t>Shikigami</t>
   </si>
   <si>
@@ -372,6 +369,12 @@
   </si>
   <si>
     <t>Melee Weapon</t>
+  </si>
+  <si>
+    <t>Reacting</t>
+  </si>
+  <si>
+    <t>Weapon</t>
   </si>
 </sst>
 </file>
@@ -800,7 +803,7 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,13 +861,13 @@
         <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>9</v>
@@ -878,75 +881,75 @@
         <v>0</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" t="s">
         <v>72</v>
       </c>
-      <c r="B4" t="s">
-        <v>73</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -960,31 +963,31 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
         <v>30</v>
       </c>
-      <c r="G5" t="s">
-        <v>31</v>
-      </c>
       <c r="H5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -998,31 +1001,31 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1033,34 +1036,34 @@
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1068,31 +1071,31 @@
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J8" t="s">
         <v>11</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L8" t="s">
         <v>11</v>
@@ -1103,31 +1106,31 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" t="s">
+        <v>82</v>
+      </c>
+      <c r="I9" t="s">
+        <v>84</v>
+      </c>
+      <c r="J9" t="s">
         <v>35</v>
       </c>
-      <c r="H9" t="s">
-        <v>83</v>
-      </c>
-      <c r="I9" t="s">
-        <v>85</v>
-      </c>
-      <c r="J9" t="s">
-        <v>36</v>
-      </c>
       <c r="K9" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1135,22 +1138,22 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1158,16 +1161,16 @@
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1175,13 +1178,13 @@
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E12" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="13" t="s">
         <v>90</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1189,135 +1192,138 @@
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1336,7 +1342,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,7 +1355,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1357,22 +1363,22 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="D3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1383,25 +1389,25 @@
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(B3,Sheet1!C$3:C$38,0))</f>
         <v>3</v>
       </c>
-      <c r="C4" s="8" t="str">
+      <c r="C4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C3,Sheet1!D$3:D$38,0))</f>
-        <v>Z</v>
-      </c>
-      <c r="D4" s="8" t="str">
+        <v>8</v>
+      </c>
+      <c r="D4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(D3,Sheet1!E$3:E$38,0))</f>
-        <v>Z</v>
+        <v>9</v>
       </c>
       <c r="E4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(E3,Sheet1!F$3:F$38,0))</f>
-        <v>5</v>
-      </c>
-      <c r="F4" s="8" t="str">
+        <v>3</v>
+      </c>
+      <c r="F4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(F3,Sheet1!G$3:G$38,0))</f>
-        <v>Z</v>
+        <v>0</v>
       </c>
       <c r="I4" t="str">
         <f>_xlfn.CONCAT(A4:F4)</f>
-        <v>13ZZ5Z</v>
+        <v>138930</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1409,13 +1415,13 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1424,7 +1430,7 @@
       </c>
       <c r="B6" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(B5,Sheet1!I$3:I$38,0))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C5,Sheet1!J$3:J$38,0))</f>
@@ -1435,7 +1441,7 @@
       <c r="F6" s="8"/>
       <c r="I6" t="str">
         <f>_xlfn.CONCAT(A6:F6)</f>
-        <v>210</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1443,13 +1449,13 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1557,12 +1563,12 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -1570,80 +1576,80 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E3" s="19"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>106</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="14" t="s">
         <v>106</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first set of weapons tested
</commit_message>
<xml_diff>
--- a/Onmyoji Modifiers.xlsx
+++ b/Onmyoji Modifiers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8C39DB-7443-4E50-BC83-52A54A0DE0B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59D9E28-91DD-4884-ACED-E83974AAD00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="114">
   <si>
     <t>Attack</t>
   </si>
@@ -375,6 +375,9 @@
   </si>
   <si>
     <t>Weapon</t>
+  </si>
+  <si>
+    <t>Critical</t>
   </si>
 </sst>
 </file>
@@ -802,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25B2E206-CE3A-441E-9767-B84A47E2A9DA}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1210,6 +1213,9 @@
       <c r="A15" s="5" t="s">
         <v>47</v>
       </c>
+      <c r="G15" s="13" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -1341,8 +1347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8DFB6C6-09DB-4B15-801E-5605D6167238}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1369,13 +1375,13 @@
         <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>74</v>
+        <v>113</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>73</v>
@@ -1393,21 +1399,21 @@
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C3,Sheet1!D$3:D$38,0))</f>
         <v>8</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="8" t="str">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(D3,Sheet1!E$3:E$38,0))</f>
-        <v>9</v>
+        <v>Z</v>
       </c>
       <c r="E4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(E3,Sheet1!F$3:F$38,0))</f>
-        <v>3</v>
-      </c>
-      <c r="F4" s="8">
+        <v>5</v>
+      </c>
+      <c r="F4" s="8" t="str">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(F3,Sheet1!G$3:G$38,0))</f>
-        <v>0</v>
+        <v>B</v>
       </c>
       <c r="I4" t="str">
         <f>_xlfn.CONCAT(A4:F4)</f>
-        <v>138930</v>
+        <v>138Z5B</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add proper mods and extremeties to dodge
</commit_message>
<xml_diff>
--- a/Onmyoji Modifiers.xlsx
+++ b/Onmyoji Modifiers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59D9E28-91DD-4884-ACED-E83974AAD00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFB00C2-4DFD-49F4-9BC6-559FF0EA401C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6E74D7C0-87F2-489D-A6BC-17043CCA5948}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25B2E206-CE3A-441E-9767-B84A47E2A9DA}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,8 +1347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8DFB6C6-09DB-4B15-801E-5605D6167238}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,16 +1372,16 @@
         <v>112</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
         <v>72</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>113</v>
+        <v>33</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>73</v>
@@ -1395,9 +1395,9 @@
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(B3,Sheet1!C$3:C$38,0))</f>
         <v>3</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="8" t="str">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C3,Sheet1!D$3:D$38,0))</f>
-        <v>8</v>
+        <v>Z</v>
       </c>
       <c r="D4" s="8" t="str">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(D3,Sheet1!E$3:E$38,0))</f>
@@ -1405,15 +1405,15 @@
       </c>
       <c r="E4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(E3,Sheet1!F$3:F$38,0))</f>
-        <v>5</v>
-      </c>
-      <c r="F4" s="8" t="str">
+        <v>3</v>
+      </c>
+      <c r="F4" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(F3,Sheet1!G$3:G$38,0))</f>
-        <v>B</v>
+        <v>4</v>
       </c>
       <c r="I4" t="str">
         <f>_xlfn.CONCAT(A4:F4)</f>
-        <v>138Z5B</v>
+        <v>13ZZ34</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1424,7 +1424,7 @@
         <v>91</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>73</v>
@@ -1440,14 +1440,14 @@
       </c>
       <c r="C6" s="8">
         <f>INDEX(Sheet1!$A$3:$A$38,MATCH(C5,Sheet1!J$3:J$38,0))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="I6" t="str">
         <f>_xlfn.CONCAT(A6:F6)</f>
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>